<commit_message>
upd. vectors of movement
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/vector of movement-3.xlsx
+++ b/migforecasting/clustering/vector of movement-3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
   <si>
     <t>oktmo</t>
   </si>
@@ -165,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +175,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -306,7 +312,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -609,15 +619,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T73"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="O71" sqref="O71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -4952,7 +4964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E70" s="2">
         <f>E67+E69</f>
         <v>-2</v>
@@ -5018,152 +5030,203 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D71" s="3" t="s">
+    <row r="71" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T71" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D72" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E71" s="10">
+      <c r="E72" s="10">
         <f>COUNTIF(E3:E70, 2)</f>
         <v>1</v>
       </c>
-      <c r="F71" s="8">
-        <f t="shared" ref="F71:T71" si="241">COUNTIF(F3:F70, 2)</f>
+      <c r="F72" s="8">
+        <f>COUNTIF(F3:F70, 2)</f>
         <v>4</v>
       </c>
-      <c r="G71" s="5">
-        <f t="shared" si="241"/>
+      <c r="G72" s="5">
+        <f>COUNTIF(G3:G70, 2)</f>
         <v>2</v>
       </c>
-      <c r="H71" s="10">
-        <f t="shared" si="241"/>
-        <v>1</v>
-      </c>
-      <c r="I71" s="10">
-        <f t="shared" si="241"/>
+      <c r="H72" s="10">
+        <f>COUNTIF(H3:H70, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="I72" s="10">
+        <f>COUNTIF(I3:I70, 2)</f>
         <v>3</v>
       </c>
-      <c r="J71" s="10">
-        <f t="shared" si="241"/>
-        <v>0</v>
-      </c>
-      <c r="K71" s="5">
-        <f t="shared" si="241"/>
+      <c r="J72" s="10">
+        <f>COUNTIF(J3:J70, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="K72" s="5">
+        <f>COUNTIF(K3:K70, 2)</f>
         <v>2</v>
       </c>
-      <c r="L71" s="5">
-        <f t="shared" si="241"/>
+      <c r="L72" s="5">
+        <f>COUNTIF(L3:L70, 2)</f>
         <v>2</v>
       </c>
-      <c r="M71" s="8">
-        <f t="shared" si="241"/>
-        <v>1</v>
-      </c>
-      <c r="N71" s="8">
-        <f t="shared" si="241"/>
+      <c r="M72" s="8">
+        <f>COUNTIF(M3:M70, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="N72" s="8">
+        <f>COUNTIF(N3:N70, 2)</f>
         <v>4</v>
       </c>
-      <c r="O71" s="8">
-        <f t="shared" si="241"/>
+      <c r="O72" s="8">
+        <f>COUNTIF(O3:O70, 2)</f>
         <v>3</v>
       </c>
-      <c r="P71" s="8">
-        <f t="shared" si="241"/>
+      <c r="P72" s="8">
+        <f>COUNTIF(P3:P70, 2)</f>
         <v>4</v>
       </c>
-      <c r="Q71" s="5">
-        <f t="shared" si="241"/>
+      <c r="Q72" s="5">
+        <f>COUNTIF(Q3:Q70, 2)</f>
         <v>3</v>
       </c>
-      <c r="R71" s="10">
-        <f t="shared" si="241"/>
+      <c r="R72" s="10">
+        <f>COUNTIF(R3:R70, 2)</f>
         <v>2</v>
       </c>
-      <c r="S71" s="8">
-        <f t="shared" si="241"/>
-        <v>0</v>
-      </c>
-      <c r="T71" s="11">
-        <f t="shared" si="241"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="4" t="s">
+      <c r="S72" s="8">
+        <f>COUNTIF(S3:S70, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="T72" s="11">
+        <f>COUNTIF(T3:T70, 2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D73" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E72" s="7">
+      <c r="E73" s="7">
         <f>COUNTIF(E3:E70, -2)</f>
         <v>13</v>
       </c>
-      <c r="F72" s="9">
-        <f t="shared" ref="F72:T72" si="242">COUNTIF(F3:F70, -2)</f>
-        <v>1</v>
-      </c>
-      <c r="G72" s="7">
-        <f t="shared" si="242"/>
+      <c r="F73" s="9">
+        <f>COUNTIF(F3:F70, -2)</f>
+        <v>1</v>
+      </c>
+      <c r="G73" s="7">
+        <f>COUNTIF(G3:G70, -2)</f>
         <v>4</v>
       </c>
-      <c r="H72" s="7">
-        <f t="shared" si="242"/>
+      <c r="H73" s="7">
+        <f>COUNTIF(H3:H70, -2)</f>
         <v>5</v>
       </c>
-      <c r="I72" s="7">
-        <f t="shared" si="242"/>
+      <c r="I73" s="7">
+        <f>COUNTIF(I3:I70, -2)</f>
         <v>6</v>
       </c>
-      <c r="J72" s="7">
-        <f t="shared" si="242"/>
+      <c r="J73" s="7">
+        <f>COUNTIF(J3:J70, -2)</f>
         <v>5</v>
       </c>
-      <c r="K72" s="7">
-        <f t="shared" si="242"/>
+      <c r="K73" s="7">
+        <f>COUNTIF(K3:K70, -2)</f>
         <v>3</v>
       </c>
-      <c r="L72" s="7">
-        <f t="shared" si="242"/>
+      <c r="L73" s="7">
+        <f>COUNTIF(L3:L70, -2)</f>
         <v>4</v>
       </c>
-      <c r="M72" s="7">
-        <f t="shared" si="242"/>
-        <v>1</v>
-      </c>
-      <c r="N72" s="6">
-        <f t="shared" si="242"/>
+      <c r="M73" s="7">
+        <f>COUNTIF(M3:M70, -2)</f>
+        <v>1</v>
+      </c>
+      <c r="N73" s="6">
+        <f>COUNTIF(N3:N70, -2)</f>
         <v>3</v>
       </c>
-      <c r="O72" s="9">
-        <f t="shared" si="242"/>
-        <v>0</v>
-      </c>
-      <c r="P72" s="6">
-        <f t="shared" si="242"/>
+      <c r="O73" s="9">
+        <f>COUNTIF(O3:O70, -2)</f>
+        <v>0</v>
+      </c>
+      <c r="P73" s="6">
+        <f>COUNTIF(P3:P70, -2)</f>
         <v>2</v>
       </c>
-      <c r="Q72" s="7">
-        <f t="shared" si="242"/>
+      <c r="Q73" s="7">
+        <f>COUNTIF(Q3:Q70, -2)</f>
         <v>4</v>
       </c>
-      <c r="R72" s="7">
-        <f t="shared" si="242"/>
+      <c r="R73" s="7">
+        <f>COUNTIF(R3:R70, -2)</f>
         <v>5</v>
       </c>
-      <c r="S72" s="7">
-        <f t="shared" si="242"/>
-        <v>0</v>
-      </c>
-      <c r="T72" s="12">
-        <f t="shared" si="242"/>
+      <c r="S73" s="7">
+        <f>COUNTIF(S3:S70, -2)</f>
+        <v>0</v>
+      </c>
+      <c r="T73" s="12">
+        <f>COUNTIF(T3:T70, -2)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="R73" s="13"/>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="O74" s="15"/>
+      <c r="R74" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:T69">

</xml_diff>